<commit_message>
Image diff and Google Chrome Portable now works.
</commit_message>
<xml_diff>
--- a/resources/images/Baseline.xlsx
+++ b/resources/images/Baseline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F62D9C-03FF-4708-878D-85B39E290541}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091A92D2-96F0-4F05-98A6-10C7B8158FFA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,21 +75,21 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>153828</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>33813</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2FF8076-2E61-4205-B2CF-18B968DB0898}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DBDB101-73EB-494B-B6D2-E376F4102AD9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -111,8 +111,58 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4267200" y="2194560"/>
-          <a:ext cx="10058400" cy="4908708"/>
+          <a:off x="4267200" y="1828800"/>
+          <a:ext cx="10058400" cy="4971573"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>33813</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B56AA5B-10E4-482F-8AC0-0EDFF7137072}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="9509760"/>
+          <a:ext cx="10058400" cy="4971573"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -389,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>